<commit_message>
update data and fix non-str data error
</commit_message>
<xml_diff>
--- a/input/new_data.xlsx
+++ b/input/new_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Đại học\học kì 6\ml\MachineLearningAssignment\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32799F06-7B54-4A5B-882F-FEA4EBBFF229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B93D10-3F31-4826-A39B-75EFB29BAFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <t>Text</t>
   </si>
   <si>
-    <t>New text data about Manchester United and other Premier League clubs.</t>
+    <t>Hibernian duo Lewis Stevenson and Paul Hanlon will leave Easter Road at the end of the summer, after almost two decades.</t>
   </si>
 </sst>
 </file>
@@ -351,7 +351,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>